<commit_message>
CV, pantalla de pagos aumentar los datos del valor del comprobante, pantallde cuentas por cobrar arreglar totales, y reporte de resumen
</commit_message>
<xml_diff>
--- a/FALEC-w1-core-web/WebContent/reportes/FALECPV-CuentaCobrar.xlsx
+++ b/FALEC-w1-core-web/WebContent/reportes/FALECPV-CuentaCobrar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/projects/gitrepositorio/FacturaElectronica-App/FALEC-w1-core-web/WebContent/reportes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17DBECEE-ECB0-0E44-8290-BFC5D24BBC2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6492B60-B8B2-EF42-8959-2913991609E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4700" yWindow="8980" windowWidth="42320" windowHeight="20280" xr2:uid="{E9788733-D204-D84A-A824-443E01B2DF94}"/>
   </bookViews>
@@ -66,9 +66,6 @@
     <t>ABONO</t>
   </si>
   <si>
-    <t>SALDO</t>
-  </si>
-  <si>
     <t>VENCIMIENTO</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>VENCIDO :</t>
+  </si>
+  <si>
+    <t>CRÉDITO</t>
   </si>
 </sst>
 </file>
@@ -170,6 +170,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -179,7 +180,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,7 +497,7 @@
   <dimension ref="A2:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -516,30 +516,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
       <c r="G4" s="3"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -549,39 +549,39 @@
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="A6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="A7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
       <c r="G7" s="3"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -613,16 +613,16 @@
         <v>6</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>